<commit_message>
fixed the script & re ran all reports
</commit_message>
<xml_diff>
--- a/PPR0.xlsx
+++ b/PPR0.xlsx
@@ -371,22 +371,22 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>ADV_PRC</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>RET_PRC</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>PRC1</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>ST</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>ADV_PRC</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>RET_PRC</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>PRC1</t>
         </is>
       </c>
     </row>

</xml_diff>